<commit_message>
analysis with ethnic minority as covariate
</commit_message>
<xml_diff>
--- a/results/mod2.galtan_corrupt.galtan.eff.MN.xlsx
+++ b/results/mod2.galtan_corrupt.galtan.eff.MN.xlsx
@@ -410,25 +410,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0901932401234611</v>
+        <v>0.0898550975333272</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0316859160841062</v>
+        <v>0.0316886475803865</v>
       </c>
       <c r="D2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0280899857814546</v>
+        <v>0.0277464895569875</v>
       </c>
       <c r="F2" t="n">
-        <v>0.152296494465468</v>
+        <v>0.151963705509667</v>
       </c>
       <c r="G2" t="n">
-        <v>2.84647727665676</v>
+        <v>2.83556113606258</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00442058840695009</v>
+        <v>0.0045745258726248</v>
       </c>
     </row>
     <row r="3">
@@ -436,25 +436,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.106051788209553</v>
+        <v>-0.107889000538331</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0721027264698347</v>
+        <v>0.0720581427078311</v>
       </c>
       <c r="D3" t="e">
         <v>#NUM!</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.247370535277572</v>
+        <v>-0.249120365038528</v>
       </c>
       <c r="F3" t="n">
-        <v>0.035266958858466</v>
+        <v>0.0333423639618653</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.47084296810775</v>
+        <v>-1.49724925572646</v>
       </c>
       <c r="H3" t="n">
-        <v>0.141333589192054</v>
+        <v>0.134328413240054</v>
       </c>
     </row>
     <row r="4">
@@ -462,25 +462,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0335091529217141</v>
+        <v>-0.0322218945184243</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0317206266096062</v>
+        <v>0.0317183223604764</v>
       </c>
       <c r="D4" t="e">
         <v>#NUM!</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.0956804386435851</v>
+        <v>-0.0943886639949896</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0286621328001569</v>
+        <v>0.029944874958141</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.05638370055295</v>
+        <v>-1.01587638060503</v>
       </c>
       <c r="H4" t="n">
-        <v>0.29079294962424</v>
+        <v>0.309688257683836</v>
       </c>
     </row>
     <row r="5">
@@ -488,25 +488,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0493677010078059</v>
+        <v>0.0502557975234283</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0268937197618372</v>
+        <v>0.0268858181835791</v>
       </c>
       <c r="D5" t="e">
         <v>#NUM!</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.00334302113570819</v>
+        <v>-0.00243943781127885</v>
       </c>
       <c r="F5" t="n">
-        <v>0.10207842315132</v>
+        <v>0.102951032858136</v>
       </c>
       <c r="G5" t="n">
-        <v>1.83565908490873</v>
+        <v>1.86923072901396</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0664080927456115</v>
+        <v>0.0615907207859216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>